<commit_message>
wip: updated mutations queries
</commit_message>
<xml_diff>
--- a/graphql/db/firms.xlsx
+++ b/graphql/db/firms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mihaildorohovic/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mihaildorohovic/Projects/stopover_project/stopover/graphql/db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A5B788-5529-C244-8F98-4C83DC144D2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25E390E-A0CE-A642-9EF0-86743920302F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2140" yWindow="5620" windowWidth="36960" windowHeight="23500" xr2:uid="{F511BAAE-9F4E-6449-883C-8219489E5E31}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="36880" windowHeight="23500" xr2:uid="{F511BAAE-9F4E-6449-883C-8219489E5E31}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -112,9 +112,6 @@
     <t>petr.novak@wildwheeladventures.cz</t>
   </si>
   <si>
-    <t>+420 123 456 789</t>
-  </si>
-  <si>
     <t>www.wildwheeladventures.cz</t>
   </si>
   <si>
@@ -136,9 +133,6 @@
     <t>info@glidequesttours.cz</t>
   </si>
   <si>
-    <t>+420 987 654 321</t>
-  </si>
-  <si>
     <t>www.glidequesttours.cz</t>
   </si>
   <si>
@@ -158,6 +152,12 @@
   </si>
   <si>
     <t>glide-quest</t>
+  </si>
+  <si>
+    <t>+420602456789</t>
+  </si>
+  <si>
+    <t>+420602654321</t>
   </si>
 </sst>
 </file>
@@ -208,19 +208,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -538,9 +534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76EAAC2D-F2F6-2E43-B9A1-6F8B09B3D0E6}">
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="408" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -562,141 +556,135 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
-        <v>34</v>
+      <c r="P1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="404" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="H2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="K2" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2" t="s">
+      <c r="L2" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M2" s="2">
+      <c r="M2">
         <v>10</v>
       </c>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2" t="s">
+      <c r="O2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2" t="s">
         <v>33</v>
-      </c>
-      <c r="P2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="340" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="H3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="I3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="4" t="s">
+      <c r="M3">
+        <v>15</v>
+      </c>
+      <c r="O3" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="M3" s="2">
-        <v>15</v>
-      </c>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>36</v>
+      <c r="P3" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wip: updated mutations queries (#184)
* wip: updated mutations queries

* wip: updated update event form

* wip: fixed yup issues
</commit_message>
<xml_diff>
--- a/graphql/db/firms.xlsx
+++ b/graphql/db/firms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mihaildorohovic/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mihaildorohovic/Projects/stopover_project/stopover/graphql/db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A5B788-5529-C244-8F98-4C83DC144D2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25E390E-A0CE-A642-9EF0-86743920302F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2140" yWindow="5620" windowWidth="36960" windowHeight="23500" xr2:uid="{F511BAAE-9F4E-6449-883C-8219489E5E31}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="36880" windowHeight="23500" xr2:uid="{F511BAAE-9F4E-6449-883C-8219489E5E31}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -112,9 +112,6 @@
     <t>petr.novak@wildwheeladventures.cz</t>
   </si>
   <si>
-    <t>+420 123 456 789</t>
-  </si>
-  <si>
     <t>www.wildwheeladventures.cz</t>
   </si>
   <si>
@@ -136,9 +133,6 @@
     <t>info@glidequesttours.cz</t>
   </si>
   <si>
-    <t>+420 987 654 321</t>
-  </si>
-  <si>
     <t>www.glidequesttours.cz</t>
   </si>
   <si>
@@ -158,6 +152,12 @@
   </si>
   <si>
     <t>glide-quest</t>
+  </si>
+  <si>
+    <t>+420602456789</t>
+  </si>
+  <si>
+    <t>+420602654321</t>
   </si>
 </sst>
 </file>
@@ -208,19 +208,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -538,9 +534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76EAAC2D-F2F6-2E43-B9A1-6F8B09B3D0E6}">
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="408" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -562,141 +556,135 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
-        <v>34</v>
+      <c r="P1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="404" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="H2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="K2" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2" t="s">
+      <c r="L2" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M2" s="2">
+      <c r="M2">
         <v>10</v>
       </c>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2" t="s">
+      <c r="O2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2" t="s">
         <v>33</v>
-      </c>
-      <c r="P2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="340" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="H3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="I3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="4" t="s">
+      <c r="M3">
+        <v>15</v>
+      </c>
+      <c r="O3" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="M3" s="2">
-        <v>15</v>
-      </c>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>36</v>
+      <c r="P3" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wip: changed firms/users seed
</commit_message>
<xml_diff>
--- a/graphql/db/firms.xlsx
+++ b/graphql/db/firms.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mihaildorohovic/Projects/stopover_project/stopover/graphql/db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25E390E-A0CE-A642-9EF0-86743920302F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1850CF36-DEA8-FF4C-9E4E-455C17F26DE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="36880" windowHeight="23500" xr2:uid="{F511BAAE-9F4E-6449-883C-8219489E5E31}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="94">
   <si>
     <t>title</t>
   </si>
@@ -83,81 +83,282 @@
     <t>business_type</t>
   </si>
   <si>
-    <t>GlideQuest Tours</t>
-  </si>
-  <si>
-    <t>GlideQuest Tours is an exhilarating and unforgettable experience for adventure enthusiasts seeking to soar through the skies and embrace the beauty of nature from a unique perspective. Our tours offer the thrilling opportunity to glide effortlessly above breathtaking landscapes, taking in panoramic views and immersing yourself in the serenity of flight.
-At GlideQuest Tours, we believe in providing our guests with a safe, professional, and personalized adventure. Our experienced and certified glider pilots ensure your comfort and security throughout the journey, making sure you can relax and fully enjoy the awe-inspiring experience of gliding.
-Whether you're a seasoned glider or a first-time flyer, our tours cater to all skill levels and preferences. We offer a range of flight options, from gentle glides over picturesque countryside to more dynamic rides showcasing the rugged beauty of mountains and coastlines. Each tour is carefully crafted to provide an unforgettable blend of adrenaline-pumping excitement and tranquility.
-As you soar through the sky, you'll witness the world from a new vantage point, spotting wildlife, landmarks, and natural wonders that are inaccessible from the ground. Our knowledgeable pilots are also passionate about sharing their expertise, pointing out interesting facts and stories about the areas you'll be flying over, adding an educational element to your adventure.
-GlideQuest Tours values sustainability and conservation. We operate with a deep respect for the environment and promote responsible flying practices. We strive to minimize our ecological footprint and raise awareness about the importance of preserving our planet's natural treasures.
-Join us at GlideQuest Tours and embark on an extraordinary journey through the air. Unleash your spirit of adventure, embrace the freedom of flight, and create memories that will last a lifetime. Get ready to glide into the unknown and let the winds guide you on an incredible quest of discovery.</t>
-  </si>
-  <si>
-    <t>WildWheel Adventures</t>
-  </si>
-  <si>
-    <t>WildWheel Adventures offers an adrenaline-fueled and unforgettable experience for thrill-seekers and outdoor enthusiasts who crave the excitement of off-road exploration. Our ATV tours provide the perfect opportunity to unleash your adventurous spirit and discover the untamed beauty of nature in a thrilling and exhilarating way.
-At WildWheel Adventures, we pride ourselves on delivering top-notch experiences that combine heart-pounding action with breathtaking scenery. Our knowledgeable and experienced guides lead you on an off-road journey through rugged terrains, taking you to hidden gems and scenic vistas that are off the beaten path.
-Whether you're a seasoned ATV rider or a beginner, our tours cater to all skill levels, ensuring a safe and enjoyable adventure for everyone. Our fleet of well-maintained and reliable ATVs are designed to tackle various terrains, including rocky trails, muddy paths, and steep inclines, providing you with the ultimate off-road experience.
-As you embark on a WildWheel adventure, you'll feel the rush of freedom as you navigate through forests, traverse through riverbeds, and conquer challenging obstacles along the way. Our tours are carefully crafted to showcase the natural beauty of the surrounding landscapes, from rolling hills and dense forests to breathtaking mountain ranges and picturesque valleys.
-Safety is our top priority at WildWheel Adventures. Our expert guides provide thorough instructions on ATV operation and safety protocols before each tour, ensuring that you have the necessary knowledge and skills to enjoy the adventure responsibly. We also provide all the necessary safety gear, including helmets, goggles, and protective equipment, to ensure your well-being throughout the journey.
-At WildWheel Adventures, we believe in sustainable tourism and responsible off-road practices. We respect the environment and promote the preservation of natural habitats. Our guides educate guests about the importance of preserving the ecosystems we explore, fostering a sense of stewardship and appreciation for the wilderness.
-Whether you're seeking an adrenaline rush, a unique outdoor experience, or simply a break from the ordinary, WildWheel Adventures has the perfect ATV tour for you. Join us as we rev up our engines and embark on an unforgettable journey through the wild, leaving behind the constraints of civilization and immersing ourselves in the untamed beauty of nature. Get ready to conquer the wilderness and create memories that will last a lifetime with WildWheel Adventures.</t>
-  </si>
-  <si>
-    <t>Petr Novák</t>
-  </si>
-  <si>
-    <t>petr.novak@wildwheeladventures.cz</t>
-  </si>
-  <si>
-    <t>www.wildwheeladventures.cz</t>
-  </si>
-  <si>
-    <t>Czechia</t>
-  </si>
-  <si>
-    <t>Prague</t>
-  </si>
-  <si>
-    <t>Main Street</t>
-  </si>
-  <si>
-    <t>WildWheel Adventures, Main Street 10, Prague, Czechia</t>
-  </si>
-  <si>
-    <t>Martina Novotná</t>
-  </si>
-  <si>
-    <t>info@glidequesttours.cz</t>
-  </si>
-  <si>
-    <t>www.glidequesttours.cz</t>
-  </si>
-  <si>
-    <t>GlideQuest Tours, Riverside Avenue 15, Prague, Czechia</t>
-  </si>
-  <si>
-    <t>Riverside Avenue</t>
-  </si>
-  <si>
     <t>individual</t>
   </si>
   <si>
     <t>ref_number</t>
   </si>
   <si>
-    <t>wild-whieel</t>
-  </si>
-  <si>
-    <t>glide-quest</t>
-  </si>
-  <si>
-    <t>+420602456789</t>
-  </si>
-  <si>
-    <t>+420602654321</t>
+    <t>Strange World Tour</t>
+  </si>
+  <si>
+    <t>Serbian Adventure Factory</t>
+  </si>
+  <si>
+    <t>Cruising Belgrade CB&amp;Co</t>
+  </si>
+  <si>
+    <t>Serbia with Love</t>
+  </si>
+  <si>
+    <t>Lokafy</t>
+  </si>
+  <si>
+    <t>V Travel Ltd</t>
+  </si>
+  <si>
+    <t>Bultrips</t>
+  </si>
+  <si>
+    <t>Serbia Tour Operator</t>
+  </si>
+  <si>
+    <t>Balkan roads d.o.o</t>
+  </si>
+  <si>
+    <t>Serbia Excursions</t>
+  </si>
+  <si>
+    <t>VICTOR TOURS</t>
+  </si>
+  <si>
+    <t>Step into the enchanting world of the Balkans with Strange World Tour, your trusted travel partner in this mysterious and captivating region. As specialists in the Balkan Peninsula, we pride ourselves on offering a range of meticulously curated travel experiences, from immersive full-day excursions to extensive multi-day adventures and seamless long-distance transfers.
+Our tours are more than just sightseeing; they are a journey into the heart of the Balkans. Dive deep into its rich history, embrace its diverse cultures, and relish its unique flavors. With every destination, we aim to offer a profound understanding of the Balkan Peninsula, allowing our guests to truly connect with the places they visit.
+At Strange World Tour, we believe that travel is not just about visiting places, but about experiencing them. We invite you to join us on a voyage of discovery, where the real joy of travel comes alive.</t>
+  </si>
+  <si>
+    <t>Dong Wang</t>
+  </si>
+  <si>
+    <t>strangeworldtour@stopoverx.com</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>strange-world-tour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Established in the vibrant spring of 2018, the Serbian Adventure Factory is not your ordinary travel entity. Our mission? To unveil a Belgrade that remains a secret even to many guidebooks – a side of the city that's authentically local, untouched by the typical tourist trail.
+We take pride in leading our guests off the beaten path, guiding them to the cherished haunts where true Belgradians unwind and celebrate life. These are the spots untouched by commercialism, where genuine Serbian culture thrives, often hidden in plain sight and unknown even to many locals.
+With a dynamic background spanning years in various sectors of tourism – from hotel management, tour operations, and tourist organizations to the thrilling realm of adventure tourism – we've cultivated a unique blend of expertise. The Serbian Adventure Factory is the culmination of this rich tapestry of experiences, designed to offer you an unparalleled journey into the heart of Belgrade.
+</t>
+  </si>
+  <si>
+    <t>Tihomir Nedeljkovic</t>
+  </si>
+  <si>
+    <t>servianadventurefactory@stopoverx.com</t>
+  </si>
+  <si>
+    <t>+905546774564</t>
+  </si>
+  <si>
+    <t>Serbia</t>
+  </si>
+  <si>
+    <t>Belgrade</t>
+  </si>
+  <si>
+    <t>Takovska</t>
+  </si>
+  <si>
+    <t>serbian-adventure-factory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meet Sinisa and Vladi, the heart and soul behind Cruising Belgrade. Born and bred in the vibrant city of Belgrade, this dynamic duo boasts more than just local roots – they bring a deep-seated passion for connecting with travelers and showcasing their beloved city from a fresh, unparalleled perspective.
+With over 15 years of expertise skippering boats across the vast expanse of Europe, their love for the water is as boundless as the rivers they navigate. Sinisa and Vladi don't just guide; they immerse you in tales of adventures, sharing insights, captivating stories, and their profound knowledge of the region.
+Embark on a cruise with Cruising Belgrade and experience the iconic landmarks of Belgrade like never before. Drift along in tranquility, soaking in the sights from a unique riverine vantage point, all while nestled in the relaxed ambiance of our vessel.
+</t>
+  </si>
+  <si>
+    <t>At Serbia with Love, we're not just a travel company – we are storytellers, curators of culture, and architects of unforgettable experiences. Dedicated to the international traveler, we endeavor to weave the intricate tapestry of Serbia's charm into every tour and activity we offer.
+Our commitment goes beyond mere sightseeing. We aim to transcend expectations, ensuring that each visitor takes away moments that linger in memory, stories that echo the heart of Serbia, and impressions that are nothing short of exceptional.
+With an unwavering passion for Serbia's rich heritage and scenic beauty, we approach every tour with enthusiasm and dedication. Our personalized service ensures that each traveler feels valued, creating an ambiance where exploration meets intimacy.
+Our benchmark of success? The radiant smiles of our satisfied customers, the tales they recount, and their eagerness to spread the word about the wonders of Serbia with Love. After all, memories are our legacy, and your recommendation, our highest accolade.</t>
+  </si>
+  <si>
+    <t>Imagine strolling through a city with a friend who knows its every corner, secret alley, and hidden gem. That's the Lokafy experience. We connect you with passionate locals who share your interests, transforming traditional walking tours into personalized urban adventures.
+With a Lokafyer by your side, you won't just witness the city's highlights; you'll dive into its soul, uncovering stories and spots only a local would know. At Lokafy, we believe in immersing travelers not just within the cityscape but within its heartbeat, making you feel less like a visitor and more a part of the vibrant tapestry of life.
+Because at the heart of every journey is not just the place, but the people you meet and the connections you forge. With Lokafy, travel becomes a truly human experience.</t>
+  </si>
+  <si>
+    <t>We love to travel!</t>
+  </si>
+  <si>
+    <t>Dive into a world of rich culture and unparalleled personal touch with us. Specializing in intimate small-group tours, we pride ourselves on offering an experience that's as unique as our guests. Every traveler is treated with the utmost personal attention, ensuring that your journey is tailored just for you.
+Guided by our team of highly educated experts, each tour is a voyage of discovery, whether you're meandering through vineyards on a wine tour, feeling the thrill of the open road on a motorcycle adventure, hiking through breathtaking landscapes, or immersing yourself in the vibrant tapestry of local cultures.
+Choose from our meticulously crafted itineraries that span both day tours for a quick escapade or multi-day journeys that allow a deeper dive into the destination's essence.
+With us, every tour is more than just a trip – it's an unforgettable experience woven with passion, knowledge, and personal touch.</t>
+  </si>
+  <si>
+    <t>At Serbia Tour Operator, we are more than just travel planners – we are curators of extraordinary experiences. Situated at the crossroads of Serbia and its enchanting neighbors, we offer an expansive array of travel services tailored to partners, agencies, businesses, and explorers from every corner of the globe.
+Our seasoned team, enriched with profound knowledge of the region, stands as a testament to our unwavering commitment to delivering excellence. Whether you're seeking group tours designed for utmost comfort and enjoyment, or bespoke itineraries crafted to the unique tastes of our partners, we have the expertise to craft the perfect journey.
+But we don't stop at groups. Individual travelers seeking unique adventures are also at the heart of what we do. Whether you're in Serbia for business or leisure, lean on Serbia Tour Operator to ensure every moment and every penny is optimally spent.
+Your satisfaction is our success. Positive reviews and personal recommendations from our clients aren't just testimonials; they're our proudest accolades. Dive into our comprehensive offerings on this site, and know that we're here for you around the clock. Reach out anytime, and we'll swiftly bring your travel dreams to life.</t>
+  </si>
+  <si>
+    <t>Step into the heart of Serbia with the nation's foremost tour operator, specializing in immersive walking tours and captivating day trips. Experience the unparalleled beauty, history, and culture of this enchanting land as we guide you through its most iconic and hidden treasures. Trust in our expertise and passion to deliver unforgettable journeys, one step at a time.</t>
+  </si>
+  <si>
+    <t>A proud subsidiary of Balkan Travel Centar, Serbia Excursions stands as a beacon of premier destination management across the Balkan tapestry. As a comprehensive Destination Management Company (DMC), we embrace the entirety of the Balkans, bringing forth unmatched expertise in crafting, managing, and delivering exceptional meetings, incentive travels, conferences, exhibitions, and more.
+But we're not just about events. Dive into the soul of the Balkans with our curated activities, excursions, tours, and seamless transportation services. Our mission? To be your steadfast ally in destination management, ensuring that every detail is meticulously planned, rooted in our profound regional knowledge and organizational acumen.
+Our vision is clear: To consistently sculpt standout products and services that strike the perfect harmony between unparalleled quality and value. As champions of sustainable development, social responsibility, and ecological mindfulness, we believe in more than just business. For us, every venture is an opportunity to make a difference, to weave a legacy of positivity, and to contribute meaningfully to the world around us.</t>
+  </si>
+  <si>
+    <t>Deeply rooted in the heart of Belgrade, Victor Tours carries a legacy of passion and expertise for Serbia's unparalleled beauty and culture. Let us weave our love for this land into your travel tapestry.
+As a distinguished incoming tour operator and Destination Management Company (DMC) based in Belgrade, our years of dedication have honed our expertise across group and individual travels, incentive management, and so much more. We stand as your trusted local partner, ready to curate your perfect Serbian experience. From hand-picking the finest hotels, crafting immersive excursions, selecting seasoned tour guides to providing the best in transportation, we've got you covered.
+Innovation is our mantra, and we sculpt experiences for every theme, budget, and adventure level. Whether you're a travel agency seeking a steadfast local ally, a corporate entity aiming for a unique incentive experience, or a solo traveler eager to delve into Serbia's allure, you've found your match in Victor Tours.
+Reach out, and let us pen your Serbian narrative. Our adept, multi-lingual team awaits, eager to craft a journey that's uniquely yours. From the initial quote to the final confirmation, we promise efficiency, precision, and a journey that resonates.</t>
+  </si>
+  <si>
+    <t>Mikhail D.</t>
+  </si>
+  <si>
+    <t>cruisingbelgrade@stopoverx.com</t>
+  </si>
+  <si>
+    <t>Pavla Vujisica 92v
+11080 Belgrade-Zemun
+Serbia</t>
+  </si>
+  <si>
+    <t>Belgrade-Zemun</t>
+  </si>
+  <si>
+    <t>Pavla Vujisica 92v</t>
+  </si>
+  <si>
+    <t>cruising-belgrade</t>
+  </si>
+  <si>
+    <t>Vladimir Peskarev</t>
+  </si>
+  <si>
+    <t>serbiawithlove@stopoverx.com</t>
+  </si>
+  <si>
+    <t>Vojevodina</t>
+  </si>
+  <si>
+    <t>Novi Sad</t>
+  </si>
+  <si>
+    <t>Narodnog Fronta 48</t>
+  </si>
+  <si>
+    <t>serbia-with-love</t>
+  </si>
+  <si>
+    <t>lokafy</t>
+  </si>
+  <si>
+    <t>v-travel-ltd</t>
+  </si>
+  <si>
+    <t>bultrips</t>
+  </si>
+  <si>
+    <t>serbia-tour-operator</t>
+  </si>
+  <si>
+    <t>balkan-roads-doo</t>
+  </si>
+  <si>
+    <t>serbia-excursions</t>
+  </si>
+  <si>
+    <t>victor-tours</t>
+  </si>
+  <si>
+    <t>lokafy@stopoverx.com</t>
+  </si>
+  <si>
+    <t>vtravelltd@stopoverx.com</t>
+  </si>
+  <si>
+    <t>bultrips@stopoverx.com</t>
+  </si>
+  <si>
+    <t>serbiatouroperator@stopoverx.com</t>
+  </si>
+  <si>
+    <t>balkanroads@stopoverx.com</t>
+  </si>
+  <si>
+    <t>serbiaexcursions@stopoverx.com</t>
+  </si>
+  <si>
+    <t>victortours@stopoverx.com</t>
+  </si>
+  <si>
+    <t>Viktor Kostov</t>
+  </si>
+  <si>
+    <t>Miloš Janković</t>
+  </si>
+  <si>
+    <t>Aleksandar Jovanovic</t>
+  </si>
+  <si>
+    <t>12, Uzundzovska Str. , Fl. 3, Office 305
+1000 Sofia</t>
+  </si>
+  <si>
+    <t>zh.k. Lyulin 5
+1359 Sofia</t>
+  </si>
+  <si>
+    <t>Koste Glavinica Street 2/9
+11000 Belgrade</t>
+  </si>
+  <si>
+    <t>Room 223, Building 1, No.396, Binjiang A
+11000 Nan Jing
+Jiang Su</t>
+  </si>
+  <si>
+    <t>Takovska
+11000 Belgrade
+Serbia</t>
+  </si>
+  <si>
+    <t>Narodnog Fronta, 48
+21102 Novi Sad</t>
+  </si>
+  <si>
+    <t>1416-40 Homewood Avenue
+M4Y2K2 Toronto
+Ontario</t>
+  </si>
+  <si>
+    <t>Katanićeva 1
+11000 Belgrade
+Belgrade</t>
+  </si>
+  <si>
+    <t>Cika Ljubina 6
+11000 Belgrade</t>
+  </si>
+  <si>
+    <t>Knez Mihailova 21a
+11000 Belgrade
+Serbia</t>
+  </si>
+  <si>
+    <t>Bulgaria</t>
+  </si>
+  <si>
+    <t>Sofia</t>
+  </si>
+  <si>
+    <t>Jiang Su</t>
+  </si>
+  <si>
+    <t>Toronto</t>
+  </si>
+  <si>
+    <t>United States</t>
   </si>
 </sst>
 </file>
@@ -216,7 +417,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -532,11 +735,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76EAAC2D-F2F6-2E43-B9A1-6F8B09B3D0E6}">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="408" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="144.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -546,13 +751,14 @@
     <col min="6" max="6" width="26.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="54.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="42.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="17" x14ac:dyDescent="0.2">
@@ -602,97 +808,406 @@
         <v>14</v>
       </c>
       <c r="P1" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="404" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="153" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="H2" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="I2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" t="s">
+        <v>91</v>
+      </c>
+      <c r="O2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="170" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="H3" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="I3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="O3" t="s">
+        <v>15</v>
+      </c>
+      <c r="P3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="153" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="B4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4" t="s">
+        <v>53</v>
+      </c>
+      <c r="L4" t="s">
+        <v>54</v>
+      </c>
+      <c r="O4" t="s">
+        <v>15</v>
+      </c>
+      <c r="P4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="187" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="B5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I5" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" t="s">
+        <v>58</v>
+      </c>
+      <c r="K5" t="s">
+        <v>59</v>
+      </c>
+      <c r="L5" t="s">
+        <v>60</v>
+      </c>
+      <c r="O5" t="s">
+        <v>15</v>
+      </c>
+      <c r="P5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="119" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="B6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I6" t="s">
+        <v>93</v>
+      </c>
+      <c r="K6" t="s">
+        <v>92</v>
+      </c>
+      <c r="O6" t="s">
+        <v>15</v>
+      </c>
+      <c r="P6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I7" t="s">
+        <v>89</v>
+      </c>
+      <c r="K7" t="s">
+        <v>90</v>
+      </c>
+      <c r="O7" t="s">
+        <v>15</v>
+      </c>
+      <c r="P7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="170" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I8" t="s">
+        <v>89</v>
+      </c>
+      <c r="K8" t="s">
+        <v>90</v>
+      </c>
+      <c r="O8" t="s">
+        <v>15</v>
+      </c>
+      <c r="P8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="204" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I9" t="s">
+        <v>37</v>
+      </c>
+      <c r="J9" t="s">
+        <v>38</v>
+      </c>
+      <c r="K9" t="s">
+        <v>38</v>
+      </c>
+      <c r="O9" t="s">
+        <v>15</v>
+      </c>
+      <c r="P9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>25</v>
       </c>
-      <c r="I2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2">
-        <v>10</v>
-      </c>
-      <c r="O2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P2" t="s">
-        <v>33</v>
+      <c r="B10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J10" t="s">
+        <v>38</v>
+      </c>
+      <c r="K10" t="s">
+        <v>38</v>
+      </c>
+      <c r="O10" t="s">
+        <v>15</v>
+      </c>
+      <c r="P10" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="340" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="11" spans="1:16" ht="170" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I11" t="s">
+        <v>37</v>
+      </c>
+      <c r="J11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K11" t="s">
+        <v>38</v>
+      </c>
+      <c r="O11" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="P11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="204" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="B12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="M3">
+      <c r="H12" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I12" t="s">
+        <v>37</v>
+      </c>
+      <c r="J12" t="s">
+        <v>38</v>
+      </c>
+      <c r="K12" t="s">
+        <v>38</v>
+      </c>
+      <c r="O12" t="s">
         <v>15</v>
       </c>
-      <c r="O3" t="s">
-        <v>31</v>
-      </c>
-      <c r="P3" t="s">
-        <v>34</v>
+      <c r="P12" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="mailto:petr.novak@wildwheeladventures.cz" xr:uid="{4793DC61-7B57-EF40-BC83-4AED1B4769F9}"/>
-    <hyperlink ref="F2" r:id="rId2" display="http://www.wildwheeladventures.cz/" xr:uid="{A5744109-E720-2748-A85C-09306B46E82E}"/>
-    <hyperlink ref="D3" r:id="rId3" display="mailto:info@glidequesttours.cz" xr:uid="{F1CB2DE0-28DE-DA4A-AECD-C20AFA337A40}"/>
-    <hyperlink ref="F3" r:id="rId4" display="http://www.glidequesttours.cz/" xr:uid="{C9C8A1BB-BCB4-D34C-AED2-3F1A08667693}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{4DA3E892-554C-4244-B6D5-103BD5764519}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{68327171-3507-BA45-9F4E-4795C9E05980}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{9F8568D9-7808-0B4F-952C-1828318DDD03}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{AE6EC2AA-EF58-604D-9257-511D0A64779A}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{435D3025-8498-784E-8717-B3F3600C4874}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{2A14B8AD-10CF-3248-849F-8A6BE84D0159}"/>
+    <hyperlink ref="D9" r:id="rId7" xr:uid="{6D8F4107-1E2B-C546-BED5-A5EF52E191F7}"/>
+    <hyperlink ref="D10" r:id="rId8" xr:uid="{729A7E4A-DBB3-BE42-8FBB-1BA1C639F7CB}"/>
+    <hyperlink ref="D11" r:id="rId9" xr:uid="{80516797-7D08-7645-88D0-DF983800A983}"/>
+    <hyperlink ref="D12" r:id="rId10" xr:uid="{DC41709C-F0EE-BF46-9343-B0B9AA29E3C4}"/>
+    <hyperlink ref="D8" r:id="rId11" xr:uid="{00A5F5A6-AED3-1044-B426-58A853FB483F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>